<commit_message>
added two more excluded datasets
</commit_message>
<xml_diff>
--- a/ms/SupplementalTables.xlsx
+++ b/ms/SupplementalTables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="0" windowWidth="16960" windowHeight="17520" tabRatio="500" activeTab="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="140">
   <si>
     <t>Study Site (Reference)</t>
   </si>
@@ -586,6 +586,15 @@
       </rPr>
       <t xml:space="preserve"> Datasets that were not used in analyses, including the study site (reference), the reported diversity pattern (D: decreasing; I: Increasing; LP: low-plateau; MP: mid-peak, and No Pattern), the data scale (local or regional), and the reason(s) the study was not included (D: large portion of gradient had anthropogenic disturbance; G: sampling gaps between sites were &gt;500m; I: insufficient or no elevational diversity data; L: no sampling in the lowest 400m; M: multiple gradients or sites too far apart; P: &lt;70% of elevational gradient sampled and not primarily upper elevaitons where diversity had already decreased monotonically; R: repeated data or non-independent transect; S: sampling effort minimal or biased elevationally).</t>
     </r>
+  </si>
+  <si>
+    <t>Guyana (Lapolla 2007)</t>
+  </si>
+  <si>
+    <t>G, S</t>
+  </si>
+  <si>
+    <t>Alps, Switzerland (Reymond et al. 2013)</t>
   </si>
 </sst>
 </file>
@@ -775,9 +784,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -796,6 +802,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1148,27 +1157,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="9"/>
+      <c r="A2" s="8"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="9"/>
+      <c r="A3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="16" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" ht="21" thickBot="1">
       <c r="A5" s="1" t="s">
@@ -1843,12 +1852,12 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1867,9 +1876,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1880,666 +1891,694 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1"/>
     <row r="4" spans="1:4" ht="37" thickBot="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="A7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="C7" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="12" t="s">
+    <row r="8" spans="1:4" ht="16" thickBot="1">
+      <c r="A8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="C8" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="12" t="s">
+    <row r="9" spans="1:4" ht="16" thickBot="1">
+      <c r="A9" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="C9" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="12" t="s">
+    <row r="10" spans="1:4" ht="16" thickBot="1">
+      <c r="A10" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="C10" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="12" t="s">
+    <row r="11" spans="1:4" ht="16" thickBot="1">
+      <c r="A11" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="C11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" thickBot="1">
-      <c r="A11" s="12" t="s">
+    <row r="12" spans="1:4" ht="16" thickBot="1">
+      <c r="A12" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="C12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" thickBot="1">
-      <c r="A12" s="12" t="s">
+    <row r="13" spans="1:4" ht="16" thickBot="1">
+      <c r="A13" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="C13" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="12" t="s">
+    <row r="14" spans="1:4" ht="16" thickBot="1">
+      <c r="A14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="C14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="12" t="s">
+    <row r="15" spans="1:4" ht="16" thickBot="1">
+      <c r="A15" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="C15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="12" t="s">
+    <row r="16" spans="1:4" ht="16" thickBot="1">
+      <c r="A16" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" thickBot="1">
-      <c r="A16" s="12" t="s">
+    <row r="17" spans="1:4" ht="16" thickBot="1">
+      <c r="A17" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="C17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" thickBot="1">
-      <c r="A17" s="12" t="s">
+    <row r="18" spans="1:4" ht="16" thickBot="1">
+      <c r="A18" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="13" t="s">
+      <c r="C18" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" thickBot="1">
-      <c r="A18" s="12" t="s">
+    <row r="19" spans="1:4" ht="16" thickBot="1">
+      <c r="A19" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="13" t="s">
+      <c r="C19" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" thickBot="1">
-      <c r="A19" s="12" t="s">
+    <row r="20" spans="1:4" ht="16" thickBot="1">
+      <c r="A20" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" thickBot="1">
-      <c r="A20" s="12" t="s">
+    <row r="21" spans="1:4" ht="16" thickBot="1">
+      <c r="A21" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" thickBot="1">
-      <c r="A21" s="12" t="s">
+    <row r="22" spans="1:4" ht="16" thickBot="1">
+      <c r="A22" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="13" t="s">
+      <c r="C22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" thickBot="1">
-      <c r="A22" s="12" t="s">
+    <row r="23" spans="1:4" ht="16" thickBot="1">
+      <c r="A23" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" thickBot="1">
+      <c r="A24" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" thickBot="1">
-      <c r="A23" s="12" t="s">
+    <row r="25" spans="1:4" ht="16" thickBot="1">
+      <c r="A25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="13" t="s">
+      <c r="C25" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" thickBot="1">
-      <c r="A24" s="12" t="s">
+    <row r="26" spans="1:4" ht="16" thickBot="1">
+      <c r="A26" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="C26" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" thickBot="1">
-      <c r="A25" s="12" t="s">
+    <row r="27" spans="1:4" ht="16" thickBot="1">
+      <c r="A27" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="13" t="s">
+      <c r="C27" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" thickBot="1">
-      <c r="A26" s="12" t="s">
+    <row r="28" spans="1:4" ht="16" thickBot="1">
+      <c r="A28" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="13" t="s">
+      <c r="C28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1">
-      <c r="A27" s="12" t="s">
+    <row r="29" spans="1:4" ht="16" thickBot="1">
+      <c r="A29" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="13" t="s">
+      <c r="C29" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1">
-      <c r="A28" s="12" t="s">
+    <row r="30" spans="1:4" ht="16" thickBot="1">
+      <c r="A30" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="13" t="s">
+      <c r="C30" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1">
-      <c r="A29" s="12" t="s">
+    <row r="31" spans="1:4" ht="16" thickBot="1">
+      <c r="A31" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="13" t="s">
+      <c r="C31" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1">
-      <c r="A30" s="12" t="s">
+    <row r="32" spans="1:4" ht="16" thickBot="1">
+      <c r="A32" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="13" t="s">
+      <c r="C32" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" thickBot="1">
-      <c r="A31" s="12" t="s">
+    <row r="33" spans="1:4" ht="16" thickBot="1">
+      <c r="A33" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" thickBot="1">
-      <c r="A32" s="12" t="s">
+    <row r="34" spans="1:4" ht="16" thickBot="1">
+      <c r="A34" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="13" t="s">
+      <c r="C34" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16" thickBot="1">
-      <c r="A33" s="12" t="s">
+    <row r="35" spans="1:4" ht="16" thickBot="1">
+      <c r="A35" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="13" t="s">
+      <c r="C35" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="16" thickBot="1">
-      <c r="A34" s="12" t="s">
+    <row r="36" spans="1:4" ht="16" thickBot="1">
+      <c r="A36" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="13" t="s">
+      <c r="C36" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16" thickBot="1">
-      <c r="A35" s="12" t="s">
+    <row r="37" spans="1:4" ht="16" thickBot="1">
+      <c r="A37" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="13" t="s">
+      <c r="C37" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" thickBot="1">
-      <c r="A36" s="12" t="s">
+    <row r="38" spans="1:4" ht="16" thickBot="1">
+      <c r="A38" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D38" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="16" thickBot="1">
-      <c r="A37" s="12" t="s">
+    <row r="39" spans="1:4" ht="16" thickBot="1">
+      <c r="A39" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="13" t="s">
+      <c r="C39" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="16" thickBot="1">
-      <c r="A38" s="12" t="s">
+    <row r="40" spans="1:4" ht="16" thickBot="1">
+      <c r="A40" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="13" t="s">
+      <c r="C40" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="16" thickBot="1">
-      <c r="A39" s="12" t="s">
+    <row r="41" spans="1:4" ht="16" thickBot="1">
+      <c r="A41" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="13" t="s">
+      <c r="C41" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" thickBot="1">
-      <c r="A40" s="12" t="s">
+    <row r="42" spans="1:4" ht="16" thickBot="1">
+      <c r="A42" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="13" t="s">
+      <c r="C42" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="16" thickBot="1">
-      <c r="A41" s="12" t="s">
+    <row r="43" spans="1:4" ht="16" thickBot="1">
+      <c r="A43" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B43" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="13" t="s">
+      <c r="C43" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" thickBot="1">
-      <c r="A42" s="12" t="s">
+    <row r="44" spans="1:4" ht="16" thickBot="1">
+      <c r="A44" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="13" t="s">
+      <c r="C44" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16" thickBot="1">
-      <c r="A43" s="12" t="s">
+    <row r="45" spans="1:4" ht="16" thickBot="1">
+      <c r="A45" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C45" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D45" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" thickBot="1">
-      <c r="A44" s="12" t="s">
+    <row r="46" spans="1:4" ht="16" thickBot="1">
+      <c r="A46" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B46" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" s="13" t="s">
+      <c r="C46" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" thickBot="1">
-      <c r="A45" s="12" t="s">
+    <row r="47" spans="1:4" ht="16" thickBot="1">
+      <c r="A47" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B47" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" s="13" t="s">
+      <c r="C47" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="16" thickBot="1">
-      <c r="A46" s="12" t="s">
+    <row r="48" spans="1:4" ht="16" thickBot="1">
+      <c r="A48" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B48" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="13" t="s">
+      <c r="C48" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="16" thickBot="1">
-      <c r="A47" s="12" t="s">
+    <row r="49" spans="1:4" ht="16" thickBot="1">
+      <c r="A49" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B49" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D47" s="13" t="s">
+      <c r="C49" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16" thickBot="1">
-      <c r="A48" s="12" t="s">
+    <row r="50" spans="1:4" ht="16" thickBot="1">
+      <c r="A50" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B50" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C50" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D50" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" thickBot="1">
-      <c r="A49" s="12" t="s">
+    <row r="51" spans="1:4" ht="16" thickBot="1">
+      <c r="A51" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B51" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="13" t="s">
+      <c r="C51" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16" thickBot="1">
-      <c r="A50" s="12" t="s">
+    <row r="52" spans="1:4" ht="16" thickBot="1">
+      <c r="A52" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B52" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" s="13" t="s">
+      <c r="C52" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>